<commit_message>
traNNsformers - Approach 1 1 Updated
</commit_message>
<xml_diff>
--- a/output/result.xlsx
+++ b/output/result.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="23">
   <si>
     <t>MNIST</t>
   </si>
@@ -49,13 +49,52 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>Dataset</t>
+  </si>
+  <si>
+    <t>Layer 2</t>
+  </si>
+  <si>
+    <t>Layer 1</t>
+  </si>
+  <si>
+    <t>Layer 3</t>
+  </si>
+  <si>
+    <t>Unclustered</t>
+  </si>
+  <si>
+    <t>Clustered</t>
+  </si>
+  <si>
+    <t>MNIST (784-1200-1200-10)</t>
+  </si>
+  <si>
+    <t>SVHN (1024-1200-1200-10)</t>
+  </si>
+  <si>
+    <t>CIFAR-10 (1024-1200-1200-10)</t>
+  </si>
+  <si>
+    <t>Scheme1: Map unclustered as well as clustered synapses</t>
+  </si>
+  <si>
+    <t>ISO-TRAINING EFFORT: Analyse the number of crossbars for clustering/unclustering for traNNsformers</t>
+  </si>
+  <si>
+    <t>Conslusion: Even with less pruning in the traNNsformers than just pruning…unclustered synapses occupy a lot of crossbars.</t>
+  </si>
+  <si>
+    <t>Ratio</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -67,6 +106,21 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -92,9 +146,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -375,13 +440,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="18.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="27.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27.7109375" style="2"/>
+    <col min="2" max="2" width="21" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="27.7109375" style="2"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -389,133 +459,324 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="2">
         <v>58800</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="2">
         <v>90000</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="2">
         <v>900</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="2">
         <f>SUM(B4,C4,D4)</f>
         <v>149700</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="2">
         <f>B4/MIN(B4,B5,B6)</f>
         <v>1.9680032130664704</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="2">
         <f>C4/MIN(C4,C5,C6)</f>
         <v>2.1996285071854533</v>
       </c>
-      <c r="J4">
+      <c r="J4" s="2">
         <f>D4/MIN(D4,D5,D6)</f>
         <v>1.1320754716981132</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="2">
         <v>42316</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="2">
         <v>80162</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="2">
         <v>795</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="2">
         <f>SUM(B5,C5,D5)</f>
         <v>123273</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="2">
         <f>B5/MIN(B4,B5,B6)</f>
         <v>1.4162929245598768</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="2">
         <f>C5/MIN(C4,C5,C6)</f>
         <v>1.9591846710333365</v>
       </c>
-      <c r="J5">
+      <c r="J5" s="2">
         <f>D5/MIN(D4,D5,D6)</f>
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="2">
         <v>29878</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="2">
         <v>40916</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="2">
         <v>925</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="2">
         <f>SUM(B6,C6,D6)</f>
         <v>71719</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="2">
         <f>B6/MIN(B4,B5,B6)</f>
         <v>1</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="2">
         <f>C6/MIN(C4,C5,C6)</f>
         <v>1</v>
       </c>
-      <c r="J6">
+      <c r="J6" s="2">
         <f>D6/MIN(D4,D5,D6)</f>
         <v>1.1635220125786163</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="2">
+        <v>18786</v>
+      </c>
+      <c r="C12" s="2">
+        <v>7399</v>
+      </c>
+      <c r="D12" s="2">
+        <f>B12/C12</f>
+        <v>2.5389917556426544</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="2">
+        <v>20436</v>
+      </c>
+      <c r="C13" s="2">
+        <v>44450</v>
+      </c>
+      <c r="D13" s="2">
+        <f t="shared" ref="D13:D24" si="0">B13/C13</f>
+        <v>0.45975253093363327</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="2">
+        <v>660</v>
+      </c>
+      <c r="C14" s="2">
+        <v>256</v>
+      </c>
+      <c r="D14" s="2">
+        <f t="shared" si="0"/>
+        <v>2.578125</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="2">
+        <v>15115</v>
+      </c>
+      <c r="C17" s="2">
+        <v>13028</v>
+      </c>
+      <c r="D17" s="2">
+        <f t="shared" si="0"/>
+        <v>1.1601934295363832</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" s="2">
+        <v>28244</v>
+      </c>
+      <c r="C18" s="2">
+        <v>9398</v>
+      </c>
+      <c r="D18" s="2">
+        <f t="shared" si="0"/>
+        <v>3.0053202809108321</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19" s="2">
+        <v>580</v>
+      </c>
+      <c r="C19" s="2">
+        <v>308</v>
+      </c>
+      <c r="D19" s="2">
+        <f t="shared" si="0"/>
+        <v>1.8831168831168832</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B22" s="2">
+        <v>39527</v>
+      </c>
+      <c r="C22" s="2">
+        <v>35574</v>
+      </c>
+      <c r="D22" s="2">
+        <f t="shared" si="0"/>
+        <v>1.1111204812503515</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B23" s="2">
+        <v>31595</v>
+      </c>
+      <c r="C23" s="2">
+        <v>28179</v>
+      </c>
+      <c r="D23" s="2">
+        <f t="shared" si="0"/>
+        <v>1.1212250257283793</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B24" s="2">
+        <v>615</v>
+      </c>
+      <c r="C24" s="2">
+        <v>443</v>
+      </c>
+      <c r="D24" s="2">
+        <f t="shared" si="0"/>
+        <v>1.3882618510158014</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed the bubugs the cluster_prune_wrapperer, cluster_prune.m is deprecated.
</commit_message>
<xml_diff>
--- a/output/result.xlsx
+++ b/output/result.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="31">
   <si>
     <t>MNIST</t>
   </si>
@@ -88,6 +88,30 @@
   </si>
   <si>
     <t>Ratio</t>
+  </si>
+  <si>
+    <t>nn.cluster_base_quality_min = 0.3</t>
+  </si>
+  <si>
+    <t>nn.cluster_base_quality_min = 0.2</t>
+  </si>
+  <si>
+    <t>Conslusion: Lower base quality for xbar utilization improved the ratio of unclustered to clustered</t>
+  </si>
+  <si>
+    <t>However, #unclustered crossbars are still high.</t>
+  </si>
+  <si>
+    <t>Lower accuracy in SVHN for transformers than just pruning.</t>
+  </si>
+  <si>
+    <t>Lower pruning in SVHN and CIFAR-10</t>
+  </si>
+  <si>
+    <t>Trying a lower base quality to reduce the number of unclustered synapses and resulting crossbars</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trying a iso-accuracy pruning for prunemodes - 1 &amp; 2, by forced prune slowdown in mode 1 </t>
   </si>
 </sst>
 </file>
@@ -440,10 +464,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J25"/>
+  <dimension ref="A1:J58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="27.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -599,184 +623,510 @@
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>10</v>
+      <c r="A10" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" s="2">
-        <v>18786</v>
-      </c>
-      <c r="C12" s="2">
-        <v>7399</v>
-      </c>
-      <c r="D12" s="2">
-        <f>B12/C12</f>
-        <v>2.5389917556426544</v>
+        <v>17</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B13" s="2">
-        <v>20436</v>
+        <v>18786</v>
       </c>
       <c r="C13" s="2">
-        <v>44450</v>
+        <v>7399</v>
       </c>
       <c r="D13" s="2">
-        <f t="shared" ref="D13:D24" si="0">B13/C13</f>
-        <v>0.45975253093363327</v>
+        <f>B13/C13</f>
+        <v>2.5389917556426544</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" s="2">
+        <v>20436</v>
+      </c>
+      <c r="C14" s="2">
+        <v>44450</v>
+      </c>
+      <c r="D14" s="2">
+        <f t="shared" ref="D14:D25" si="0">B14/C14</f>
+        <v>0.45975253093363327</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B15" s="2">
         <v>660</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C15" s="2">
         <v>256</v>
       </c>
-      <c r="D14" s="2">
+      <c r="D15" s="2">
         <f t="shared" si="0"/>
         <v>2.578125</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="2">
+      <c r="B18" s="2">
         <v>15115</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C18" s="2">
         <v>13028</v>
       </c>
-      <c r="D17" s="2">
+      <c r="D18" s="2">
         <f t="shared" si="0"/>
         <v>1.1601934295363832</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B18" s="2">
+      <c r="B19" s="2">
         <v>28244</v>
       </c>
-      <c r="C18" s="2">
+      <c r="C19" s="2">
         <v>9398</v>
       </c>
-      <c r="D18" s="2">
+      <c r="D19" s="2">
         <f t="shared" si="0"/>
         <v>3.0053202809108321</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="2">
+      <c r="B20" s="2">
         <v>580</v>
       </c>
-      <c r="C19" s="2">
+      <c r="C20" s="2">
         <v>308</v>
       </c>
-      <c r="D19" s="2">
+      <c r="D20" s="2">
         <f t="shared" si="0"/>
         <v>1.8831168831168832</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B22" s="2">
+      <c r="B23" s="2">
         <v>39527</v>
       </c>
-      <c r="C22" s="2">
+      <c r="C23" s="2">
         <v>35574</v>
       </c>
-      <c r="D22" s="2">
+      <c r="D23" s="2">
         <f t="shared" si="0"/>
         <v>1.1111204812503515</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B23" s="2">
+      <c r="B24" s="2">
         <v>31595</v>
       </c>
-      <c r="C23" s="2">
+      <c r="C24" s="2">
         <v>28179</v>
       </c>
-      <c r="D23" s="2">
+      <c r="D24" s="2">
         <f t="shared" si="0"/>
         <v>1.1212250257283793</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B24" s="2">
+      <c r="B25" s="2">
         <v>615</v>
       </c>
-      <c r="C24" s="2">
+      <c r="C25" s="2">
         <v>443</v>
       </c>
-      <c r="D24" s="2">
+      <c r="D25" s="2">
         <f t="shared" si="0"/>
         <v>1.3882618510158014</v>
       </c>
     </row>
-    <row r="25" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
+    <row r="26" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
         <v>21</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B31" s="2">
+        <v>15174</v>
+      </c>
+      <c r="C31" s="2">
+        <v>8712</v>
+      </c>
+      <c r="D31" s="2">
+        <f>B31/C31</f>
+        <v>1.7417355371900827</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B32" s="2">
+        <v>13733</v>
+      </c>
+      <c r="C32" s="2">
+        <v>58605</v>
+      </c>
+      <c r="D32" s="2">
+        <f t="shared" ref="D32:D43" si="1">B32/C32</f>
+        <v>0.23433154167733128</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B33" s="2">
+        <v>542</v>
+      </c>
+      <c r="C33" s="2">
+        <v>785</v>
+      </c>
+      <c r="D33" s="2">
+        <f t="shared" si="1"/>
+        <v>0.69044585987261142</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B36" s="2">
+        <v>13414</v>
+      </c>
+      <c r="C36" s="2">
+        <v>11746</v>
+      </c>
+      <c r="D36" s="2">
+        <f t="shared" ref="D36:D43" si="2">B36/C36</f>
+        <v>1.1420057892048356</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B37" s="2">
+        <v>23899</v>
+      </c>
+      <c r="C37" s="2">
+        <v>8977</v>
+      </c>
+      <c r="D37" s="2">
+        <f t="shared" si="2"/>
+        <v>2.6622479670268464</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B38" s="2">
+        <v>496</v>
+      </c>
+      <c r="C38" s="2">
+        <v>387</v>
+      </c>
+      <c r="D38" s="2">
+        <f t="shared" si="2"/>
+        <v>1.2816537467700257</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B41" s="2">
+        <v>31179</v>
+      </c>
+      <c r="C41" s="2">
+        <v>48248</v>
+      </c>
+      <c r="D41" s="2">
+        <f t="shared" ref="D41:D43" si="3">B41/C41</f>
+        <v>0.64622367766539546</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B42" s="2">
+        <v>25075</v>
+      </c>
+      <c r="C42" s="2">
+        <v>45235</v>
+      </c>
+      <c r="D42" s="2">
+        <f t="shared" si="3"/>
+        <v>0.55432740134851333</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B43" s="2">
+        <v>502</v>
+      </c>
+      <c r="C43" s="2">
+        <v>849</v>
+      </c>
+      <c r="D43" s="2">
+        <f t="shared" si="3"/>
+        <v>0.591283863368669</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B51" s="2">
+        <v>15174</v>
+      </c>
+      <c r="C51" s="2">
+        <v>8712</v>
+      </c>
+      <c r="D51" s="2">
+        <f>B51/C51</f>
+        <v>1.7417355371900827</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B52" s="2">
+        <v>13733</v>
+      </c>
+      <c r="C52" s="2">
+        <v>58605</v>
+      </c>
+      <c r="D52" s="2">
+        <f t="shared" ref="D52:D53" si="4">B52/C52</f>
+        <v>0.23433154167733128</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B53" s="2">
+        <v>542</v>
+      </c>
+      <c r="C53" s="2">
+        <v>785</v>
+      </c>
+      <c r="D53" s="2">
+        <f t="shared" si="4"/>
+        <v>0.69044585987261142</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B56" s="2">
+        <v>31179</v>
+      </c>
+      <c r="C56" s="2">
+        <v>48248</v>
+      </c>
+      <c r="D56" s="2">
+        <f t="shared" ref="D56:D58" si="5">B56/C56</f>
+        <v>0.64622367766539546</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B57" s="2">
+        <v>25075</v>
+      </c>
+      <c r="C57" s="2">
+        <v>45235</v>
+      </c>
+      <c r="D57" s="2">
+        <f t="shared" si="5"/>
+        <v>0.55432740134851333</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B58" s="2">
+        <v>502</v>
+      </c>
+      <c r="C58" s="2">
+        <v>849</v>
+      </c>
+      <c r="D58" s="2">
+        <f t="shared" si="5"/>
+        <v>0.591283863368669</v>
       </c>
     </row>
   </sheetData>

</xml_diff>